<commit_message>
comment out other optimizer that executes after the join-order optimizer in DuckDB original code - for fair comparison
</commit_message>
<xml_diff>
--- a/chuying/visualization/2.with timer/0817test/workspace.xlsx
+++ b/chuying/visualization/2.with timer/0817test/workspace.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chuyinghe/Documents/duckdb-master-rl/chuying/visualization/2.with timer/0817test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA864471-CB24-1B45-B25A-F73C24C28AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC4BD36-D31D-2646-BB3F-4628EF9227DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="-21140" windowWidth="17000" windowHeight="19540" xr2:uid="{4BC63D49-B4F6-E248-AB4E-285880F5BF28}"/>
   </bookViews>
   <sheets>
-    <sheet name="workspace" sheetId="3" r:id="rId1"/>
-    <sheet name="header" sheetId="1" r:id="rId2"/>
+    <sheet name="RL" sheetId="3" r:id="rId1"/>
+    <sheet name="DP" sheetId="4" r:id="rId2"/>
+    <sheet name="header" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">header!$A$1:$C$114</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DP!$A$1:$C$114</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">header!$A$1:$C$114</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RL!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="126">
   <si>
     <t>Query</t>
   </si>
@@ -410,6 +413,12 @@
   </si>
   <si>
     <t>Error local-solved fixing deep copy for LogicalChunkGet</t>
+  </si>
+  <si>
+    <t>1. Run</t>
+  </si>
+  <si>
+    <t>2. Run</t>
   </si>
 </sst>
 </file>
@@ -772,22 +781,2556 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C65D470-C02B-104A-988B-0126A948A388}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2">
+        <v>0.873</v>
+      </c>
+      <c r="C2">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="C3">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="C4">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="C5">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="C7">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="C8">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="C9">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="C10">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11">
+        <v>0.48</v>
+      </c>
+      <c r="C11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12">
+        <v>0.435</v>
+      </c>
+      <c r="C12">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="C13">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14">
+        <v>0.59</v>
+      </c>
+      <c r="C14">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="C15">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16">
+        <v>1.0660000000000001</v>
+      </c>
+      <c r="C16">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="C17">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="C18">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="C19">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="C20">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="C21">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>0.85</v>
+      </c>
+      <c r="C22">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>0.64</v>
+      </c>
+      <c r="C23">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24">
+        <v>1.018</v>
+      </c>
+      <c r="C24">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25">
+        <v>3.7280000000000002</v>
+      </c>
+      <c r="C25">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26">
+        <v>3.6859999999999999</v>
+      </c>
+      <c r="C26">
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27">
+        <v>3.7360000000000002</v>
+      </c>
+      <c r="C27">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28">
+        <v>3.0350000000000001</v>
+      </c>
+      <c r="C28">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29">
+        <v>3.0310000000000001</v>
+      </c>
+      <c r="C29">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30">
+        <v>2.71</v>
+      </c>
+      <c r="C30">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31">
+        <v>2.6789999999999998</v>
+      </c>
+      <c r="C31">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32">
+        <v>3.2839999999999998</v>
+      </c>
+      <c r="C32">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33">
+        <v>3.3769999999999998</v>
+      </c>
+      <c r="C33">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34">
+        <v>2.972</v>
+      </c>
+      <c r="C34">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35">
+        <v>3.0059999999999998</v>
+      </c>
+      <c r="C35">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>0.873</v>
+      </c>
+      <c r="C36">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="C37">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="C38">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="C39">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="C40">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="C41">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="C42">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="C43">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="C44">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45">
+        <v>0.48</v>
+      </c>
+      <c r="C45">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46">
+        <v>0.435</v>
+      </c>
+      <c r="C46">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="C47">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48">
+        <v>0.59</v>
+      </c>
+      <c r="C48">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="C49">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50">
+        <v>1.0660000000000001</v>
+      </c>
+      <c r="C50">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="C51">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="C52">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B53">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="C53">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="C54">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B55">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="C55">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56">
+        <v>0.85</v>
+      </c>
+      <c r="C56">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57">
+        <v>0.64</v>
+      </c>
+      <c r="C57">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B58">
+        <v>1.018</v>
+      </c>
+      <c r="C58">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B59">
+        <v>3.7280000000000002</v>
+      </c>
+      <c r="C59">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60">
+        <v>3.6859999999999999</v>
+      </c>
+      <c r="C60">
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61">
+        <v>3.7360000000000002</v>
+      </c>
+      <c r="C61">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62">
+        <v>3.0350000000000001</v>
+      </c>
+      <c r="C62">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B63">
+        <v>3.0310000000000001</v>
+      </c>
+      <c r="C63">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B64">
+        <v>2.71</v>
+      </c>
+      <c r="C64">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B65">
+        <v>2.6789999999999998</v>
+      </c>
+      <c r="C65">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B66">
+        <v>3.2839999999999998</v>
+      </c>
+      <c r="C66">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B67">
+        <v>3.3769999999999998</v>
+      </c>
+      <c r="C67">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B68">
+        <v>2.972</v>
+      </c>
+      <c r="C68">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B69">
+        <v>3.0059999999999998</v>
+      </c>
+      <c r="C69">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B70">
+        <v>0.873</v>
+      </c>
+      <c r="C70">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B71">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="C71">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B72">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="C72">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B73">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="C73">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B74">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="C74">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B75">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="C75">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B76">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="C76">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B77">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="C77">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B78">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="C78">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B79">
+        <v>0.48</v>
+      </c>
+      <c r="C79">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B80">
+        <v>0.435</v>
+      </c>
+      <c r="C80">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B81">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="C81">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B82">
+        <v>0.59</v>
+      </c>
+      <c r="C82">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B83">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="C83">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B84">
+        <v>1.0660000000000001</v>
+      </c>
+      <c r="C84">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B85">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="C85">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B86">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="C86">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B87">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="C87">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B88">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="C88">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B89">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="C89">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B90">
+        <v>0.85</v>
+      </c>
+      <c r="C90">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B91">
+        <v>0.64</v>
+      </c>
+      <c r="C91">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B92">
+        <v>1.018</v>
+      </c>
+      <c r="C92">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B93">
+        <v>3.7280000000000002</v>
+      </c>
+      <c r="C93">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B94">
+        <v>3.6859999999999999</v>
+      </c>
+      <c r="C94">
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B95">
+        <v>3.7360000000000002</v>
+      </c>
+      <c r="C95">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B96">
+        <v>3.0350000000000001</v>
+      </c>
+      <c r="C96">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B97">
+        <v>3.0310000000000001</v>
+      </c>
+      <c r="C97">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B98">
+        <v>2.71</v>
+      </c>
+      <c r="C98">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B99">
+        <v>2.6789999999999998</v>
+      </c>
+      <c r="C99">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B100">
+        <v>3.2839999999999998</v>
+      </c>
+      <c r="C100">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B101">
+        <v>3.3769999999999998</v>
+      </c>
+      <c r="C101">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B102">
+        <v>2.972</v>
+      </c>
+      <c r="C102">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B103">
+        <v>3.0059999999999998</v>
+      </c>
+      <c r="C103">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B104">
+        <v>3.7360000000000002</v>
+      </c>
+      <c r="C104">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B105">
+        <v>3.0350000000000001</v>
+      </c>
+      <c r="C105">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B106">
+        <v>3.0310000000000001</v>
+      </c>
+      <c r="C106">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B107">
+        <v>2.71</v>
+      </c>
+      <c r="C107">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B108">
+        <v>2.6789999999999998</v>
+      </c>
+      <c r="C108">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B109">
+        <v>3.2839999999999998</v>
+      </c>
+      <c r="C109">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B110">
+        <v>3.3769999999999998</v>
+      </c>
+      <c r="C110">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B111">
+        <v>2.972</v>
+      </c>
+      <c r="C111">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B112">
+        <v>3.0059999999999998</v>
+      </c>
+      <c r="C112">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B113">
+        <v>2.972</v>
+      </c>
+      <c r="C113">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B114">
+        <v>3.0059999999999998</v>
+      </c>
+      <c r="C114">
+        <v>3.09</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{3C65D470-C02B-104A-988B-0126A948A388}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C36">
+    <sortCondition ref="A2:A36"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9010B15B-2780-4F44-B63C-77DB792E7A58}">
+  <dimension ref="A1:C114"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2">
+        <v>0.873</v>
+      </c>
+      <c r="C2">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="C3">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="C4">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="C5">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="C7">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="C8">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="C9">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="C10">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11">
+        <v>0.48</v>
+      </c>
+      <c r="C11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12">
+        <v>0.435</v>
+      </c>
+      <c r="C12">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="C13">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14">
+        <v>0.59</v>
+      </c>
+      <c r="C14">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="C15">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16">
+        <v>1.0660000000000001</v>
+      </c>
+      <c r="C16">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="C17">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="C18">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="C19">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="C20">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="C21">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>0.85</v>
+      </c>
+      <c r="C22">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>0.64</v>
+      </c>
+      <c r="C23">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24">
+        <v>1.018</v>
+      </c>
+      <c r="C24">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25">
+        <v>3.7280000000000002</v>
+      </c>
+      <c r="C25">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26">
+        <v>3.6859999999999999</v>
+      </c>
+      <c r="C26">
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27">
+        <v>3.7360000000000002</v>
+      </c>
+      <c r="C27">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28">
+        <v>3.0350000000000001</v>
+      </c>
+      <c r="C28">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29">
+        <v>3.0310000000000001</v>
+      </c>
+      <c r="C29">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30">
+        <v>2.71</v>
+      </c>
+      <c r="C30">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31">
+        <v>2.6789999999999998</v>
+      </c>
+      <c r="C31">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32">
+        <v>3.2839999999999998</v>
+      </c>
+      <c r="C32">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33">
+        <v>3.3769999999999998</v>
+      </c>
+      <c r="C33">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34">
+        <v>2.972</v>
+      </c>
+      <c r="C34">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35">
+        <v>3.0059999999999998</v>
+      </c>
+      <c r="C35">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>0.873</v>
+      </c>
+      <c r="C36">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="C37">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="C38">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="C39">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="C40">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="C41">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="C42">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="C43">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="C44">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45">
+        <v>0.48</v>
+      </c>
+      <c r="C45">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46">
+        <v>0.435</v>
+      </c>
+      <c r="C46">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="C47">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48">
+        <v>0.59</v>
+      </c>
+      <c r="C48">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="C49">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50">
+        <v>1.0660000000000001</v>
+      </c>
+      <c r="C50">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="C51">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="C52">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B53">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="C53">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="C54">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B55">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="C55">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56">
+        <v>0.85</v>
+      </c>
+      <c r="C56">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57">
+        <v>0.64</v>
+      </c>
+      <c r="C57">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B58">
+        <v>1.018</v>
+      </c>
+      <c r="C58">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B59">
+        <v>3.7280000000000002</v>
+      </c>
+      <c r="C59">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60">
+        <v>3.6859999999999999</v>
+      </c>
+      <c r="C60">
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61">
+        <v>3.7360000000000002</v>
+      </c>
+      <c r="C61">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62">
+        <v>3.0350000000000001</v>
+      </c>
+      <c r="C62">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B63">
+        <v>3.0310000000000001</v>
+      </c>
+      <c r="C63">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B64">
+        <v>2.71</v>
+      </c>
+      <c r="C64">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B65">
+        <v>2.6789999999999998</v>
+      </c>
+      <c r="C65">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B66">
+        <v>3.2839999999999998</v>
+      </c>
+      <c r="C66">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B67">
+        <v>3.3769999999999998</v>
+      </c>
+      <c r="C67">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B68">
+        <v>2.972</v>
+      </c>
+      <c r="C68">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B69">
+        <v>3.0059999999999998</v>
+      </c>
+      <c r="C69">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B70">
+        <v>0.873</v>
+      </c>
+      <c r="C70">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B71">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="C71">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B72">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="C72">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B73">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="C73">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B74">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="C74">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B75">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="C75">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B76">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="C76">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B77">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="C77">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B78">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="C78">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B79">
+        <v>0.48</v>
+      </c>
+      <c r="C79">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B80">
+        <v>0.435</v>
+      </c>
+      <c r="C80">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B81">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="C81">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B82">
+        <v>0.59</v>
+      </c>
+      <c r="C82">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B83">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="C83">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B84">
+        <v>1.0660000000000001</v>
+      </c>
+      <c r="C84">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B85">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="C85">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B86">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="C86">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B87">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="C87">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B88">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="C88">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B89">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="C89">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B90">
+        <v>0.85</v>
+      </c>
+      <c r="C90">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B91">
+        <v>0.64</v>
+      </c>
+      <c r="C91">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B92">
+        <v>1.018</v>
+      </c>
+      <c r="C92">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B93">
+        <v>3.7280000000000002</v>
+      </c>
+      <c r="C93">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B94">
+        <v>3.6859999999999999</v>
+      </c>
+      <c r="C94">
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B95">
+        <v>3.7360000000000002</v>
+      </c>
+      <c r="C95">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B96">
+        <v>3.0350000000000001</v>
+      </c>
+      <c r="C96">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B97">
+        <v>3.0310000000000001</v>
+      </c>
+      <c r="C97">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B98">
+        <v>2.71</v>
+      </c>
+      <c r="C98">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B99">
+        <v>2.6789999999999998</v>
+      </c>
+      <c r="C99">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B100">
+        <v>3.2839999999999998</v>
+      </c>
+      <c r="C100">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B101">
+        <v>3.3769999999999998</v>
+      </c>
+      <c r="C101">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B102">
+        <v>2.972</v>
+      </c>
+      <c r="C102">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B103">
+        <v>3.0059999999999998</v>
+      </c>
+      <c r="C103">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B104">
+        <v>3.7280000000000002</v>
+      </c>
+      <c r="C104">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B105">
+        <v>3.6859999999999999</v>
+      </c>
+      <c r="C105">
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B106">
+        <v>3.7360000000000002</v>
+      </c>
+      <c r="C106">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B107">
+        <v>3.0350000000000001</v>
+      </c>
+      <c r="C107">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B108">
+        <v>3.0310000000000001</v>
+      </c>
+      <c r="C108">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B109">
+        <v>2.71</v>
+      </c>
+      <c r="C109">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B110">
+        <v>2.6789999999999998</v>
+      </c>
+      <c r="C110">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B111">
+        <v>3.2839999999999998</v>
+      </c>
+      <c r="C111">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B112">
+        <v>3.3769999999999998</v>
+      </c>
+      <c r="C112">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B113">
+        <v>2.972</v>
+      </c>
+      <c r="C113">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B114">
+        <v>3.0059999999999998</v>
+      </c>
+      <c r="C114">
+        <v>3.09</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C114" xr:uid="{9010B15B-2780-4F44-B63C-77DB792E7A58}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C36">
+    <sortCondition ref="A2:A36"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F7E38B-FAA4-8B41-8AC5-88C523A72AA1}">
   <dimension ref="A1:C127"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="A16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>